<commit_message>
Add WPF and library
</commit_message>
<xml_diff>
--- a/Diagrammer/CRC-kort.xlsx
+++ b/Diagrammer/CRC-kort.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaspe\Documents\Landlyst-24062020\Diagrammer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d01a9e19b0696d5/programmering/h2/landlyst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24D33FD-26A0-4CE2-8992-551B303129F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38320882-72EC-4BEA-8949-C468A3D1E1C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Class:</t>
   </si>
@@ -48,21 +47,12 @@
     <t>Responsibilities:</t>
   </si>
   <si>
-    <t>Receptionist</t>
-  </si>
-  <si>
     <t>Check available rooms</t>
   </si>
   <si>
-    <t>Check status on rooms</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
-    <t>Change room status</t>
-  </si>
-  <si>
     <t>Reserve  a room</t>
   </si>
   <si>
@@ -81,9 +71,6 @@
     <t>Room</t>
   </si>
   <si>
-    <t>CleaningService</t>
-  </si>
-  <si>
     <t>RoomAddition</t>
   </si>
   <si>
@@ -102,15 +89,9 @@
     <t>The hotel room with its additions</t>
   </si>
   <si>
-    <t>The cleaning lady, that cleans the rooms</t>
-  </si>
-  <si>
     <t>This reception is responsable for all phone &amp; in person booking</t>
   </si>
   <si>
-    <t>Customer, Room</t>
-  </si>
-  <si>
     <t>Check Discount</t>
   </si>
   <si>
@@ -135,16 +116,73 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Reservations</t>
-  </si>
-  <si>
-    <t>Rooms</t>
+    <t>Reception</t>
+  </si>
+  <si>
+    <t>Customer, Room, resevation</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>start date</t>
+  </si>
+  <si>
+    <t>enddate</t>
+  </si>
+  <si>
+    <t>ordrenummer</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sending eamils to custormers</t>
+  </si>
+  <si>
+    <t>emailAdresse</t>
+  </si>
+  <si>
+    <t>invoice, reception</t>
+  </si>
+  <si>
+    <t>invoice</t>
+  </si>
+  <si>
+    <t>make and send invoice to custormers</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>wordapplication</t>
+  </si>
+  <si>
+    <t>Roomreception</t>
+  </si>
+  <si>
+    <t>Customer, Room, invoice</t>
+  </si>
+  <si>
+    <t>Room, reception</t>
+  </si>
+  <si>
+    <t>rooms</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>resevations</t>
+  </si>
+  <si>
+    <t>resevation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -377,6 +415,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,37 +747,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0713845-C1D6-45D3-9AA6-43204E1C6C6F}">
-  <dimension ref="B1:T48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" customWidth="1"/>
     <col min="17" max="17" width="2" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" customWidth="1"/>
+    <col min="18" max="18" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="8"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="23"/>
       <c r="E2" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -729,12 +785,12 @@
       <c r="I2" s="9"/>
       <c r="J2" s="10"/>
       <c r="L2" s="8"/>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="20"/>
+      <c r="N2" s="23"/>
       <c r="O2" s="9" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
@@ -742,14 +798,14 @@
       <c r="S2" s="9"/>
       <c r="T2" s="10"/>
     </row>
-    <row r="3" spans="2:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -757,12 +813,12 @@
       <c r="I3" s="2"/>
       <c r="J3" s="12"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="21"/>
+      <c r="N3" s="26"/>
       <c r="O3" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -770,12 +826,12 @@
       <c r="S3" s="2"/>
       <c r="T3" s="12"/>
     </row>
-    <row r="4" spans="2:20" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -783,10 +839,10 @@
       <c r="I4" s="13"/>
       <c r="J4" s="12"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="22"/>
+      <c r="N4" s="27"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
@@ -794,7 +850,7 @@
       <c r="S4" s="13"/>
       <c r="T4" s="12"/>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
       <c r="C5" s="14"/>
       <c r="D5" s="3" t="s">
@@ -822,239 +878,233 @@
       <c r="S5" s="1"/>
       <c r="T5" s="12"/>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
+      <c r="D6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="18"/>
+      <c r="H6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="24"/>
       <c r="J6" s="12"/>
       <c r="L6" s="11"/>
       <c r="M6" s="13"/>
-      <c r="N6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="19"/>
+      <c r="N6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="24"/>
+      <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="S6" s="18"/>
+      <c r="R6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="24"/>
       <c r="T6" s="12"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="11"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="18"/>
+      <c r="H7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="24"/>
       <c r="J7" s="12"/>
       <c r="L7" s="11"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="18"/>
-      <c r="P7" s="19"/>
+      <c r="N7" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="24"/>
+      <c r="P7" s="25"/>
       <c r="Q7" s="5"/>
-      <c r="R7" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7" s="18"/>
+      <c r="R7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="24"/>
       <c r="T7" s="12"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
+      <c r="D8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="12"/>
       <c r="L8" s="11"/>
       <c r="M8" s="13"/>
-      <c r="N8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" s="18"/>
-      <c r="P8" s="19"/>
+      <c r="N8" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="25"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="S8" s="18"/>
+      <c r="R8" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="24"/>
       <c r="T8" s="12"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="11"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="12"/>
       <c r="L9" s="11"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="O9" s="18"/>
-      <c r="P9" s="19"/>
+      <c r="N9" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="25"/>
       <c r="Q9" s="7"/>
-      <c r="R9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="S9" s="18"/>
+      <c r="R9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="S9" s="24"/>
       <c r="T9" s="12"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="12"/>
       <c r="L10" s="11"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="19"/>
+      <c r="N10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="25"/>
       <c r="Q10" s="5"/>
-      <c r="R10" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="S10" s="18"/>
+      <c r="R10" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="24"/>
       <c r="T10" s="12"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="12"/>
       <c r="L11" s="11"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="19"/>
+      <c r="N11" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="24"/>
+      <c r="P11" s="25"/>
       <c r="Q11" s="5"/>
-      <c r="R11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="S11" s="18"/>
+      <c r="R11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="24"/>
       <c r="T11" s="12"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="12"/>
       <c r="L12" s="11"/>
       <c r="M12" s="13"/>
-      <c r="N12" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="19"/>
+      <c r="N12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="24"/>
+      <c r="P12" s="25"/>
       <c r="Q12" s="5"/>
-      <c r="R12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="S12" s="18"/>
+      <c r="R12" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="S12" s="24"/>
       <c r="T12" s="12"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="11"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="12"/>
       <c r="L13" s="11"/>
       <c r="M13" s="13"/>
-      <c r="N13" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="O13" s="18"/>
-      <c r="P13" s="19"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="25"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="S13" s="18"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
       <c r="T13" s="12"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
       <c r="C14" s="13"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="12"/>
       <c r="L14" s="11"/>
       <c r="M14" s="13"/>
-      <c r="N14" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" s="18"/>
-      <c r="P14" s="19"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="25"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="S14" s="18"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
       <c r="T14" s="12"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15" s="11"/>
       <c r="C15" s="13"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="12"/>
       <c r="L15" s="11"/>
       <c r="M15" s="13"/>
@@ -1062,11 +1112,11 @@
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
       <c r="T15" s="12"/>
     </row>
-    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -1086,15 +1136,15 @@
       <c r="S16" s="16"/>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B18" s="8"/>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -1107,7 +1157,7 @@
       </c>
       <c r="N18" s="20"/>
       <c r="O18" s="9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
@@ -1115,14 +1165,14 @@
       <c r="S18" s="9"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="11"/>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="26"/>
       <c r="E19" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1135,7 +1185,7 @@
       </c>
       <c r="N19" s="21"/>
       <c r="O19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -1143,12 +1193,12 @@
       <c r="S19" s="2"/>
       <c r="T19" s="12"/>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="11"/>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1167,7 +1217,7 @@
       <c r="S20" s="13"/>
       <c r="T20" s="12"/>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="11"/>
       <c r="C21" s="14"/>
       <c r="D21" s="3" t="s">
@@ -1195,75 +1245,75 @@
       <c r="S21" s="1"/>
       <c r="T21" s="12"/>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="11"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
+      <c r="D22" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="25"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="18"/>
+      <c r="H22" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="24"/>
       <c r="J22" s="12"/>
       <c r="L22" s="11"/>
       <c r="M22" s="13"/>
       <c r="N22" s="18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O22" s="18"/>
       <c r="P22" s="19"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S22" s="18"/>
       <c r="T22" s="12"/>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="11"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="19"/>
+      <c r="D23" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="12"/>
       <c r="L23" s="11"/>
       <c r="M23" s="13"/>
-      <c r="N23" s="18" t="s">
-        <v>7</v>
+      <c r="N23" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="O23" s="18"/>
       <c r="P23" s="19"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="18" t="s">
-        <v>15</v>
-      </c>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="18"/>
       <c r="S23" s="18"/>
       <c r="T23" s="12"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B24" s="11"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="19"/>
+      <c r="D24" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="25"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="12"/>
       <c r="L24" s="11"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="18"/>
+      <c r="N24" s="28" t="s">
+        <v>33</v>
+      </c>
       <c r="O24" s="18"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="5"/>
@@ -1271,21 +1321,23 @@
       <c r="S24" s="18"/>
       <c r="T24" s="12"/>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B25" s="11"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="19"/>
+      <c r="D25" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="25"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="12"/>
       <c r="L25" s="11"/>
       <c r="M25" s="13"/>
-      <c r="N25" s="18"/>
+      <c r="N25" s="28" t="s">
+        <v>31</v>
+      </c>
       <c r="O25" s="18"/>
       <c r="P25" s="19"/>
       <c r="Q25" s="5"/>
@@ -1293,19 +1345,21 @@
       <c r="S25" s="18"/>
       <c r="T25" s="12"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B26" s="11"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="12"/>
       <c r="L26" s="11"/>
       <c r="M26" s="13"/>
-      <c r="N26" s="18"/>
+      <c r="N26" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="O26" s="18"/>
       <c r="P26" s="19"/>
       <c r="Q26" s="5"/>
@@ -1313,15 +1367,15 @@
       <c r="S26" s="18"/>
       <c r="T26" s="12"/>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B27" s="11"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="19"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="12"/>
       <c r="L27" s="11"/>
       <c r="M27" s="13"/>
@@ -1333,15 +1387,15 @@
       <c r="S27" s="18"/>
       <c r="T27" s="12"/>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" s="11"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="19"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="12"/>
       <c r="L28" s="11"/>
       <c r="M28" s="13"/>
@@ -1353,15 +1407,15 @@
       <c r="S28" s="18"/>
       <c r="T28" s="12"/>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B29" s="11"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="19"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="12"/>
       <c r="L29" s="11"/>
       <c r="M29" s="13"/>
@@ -1373,15 +1427,15 @@
       <c r="S29" s="18"/>
       <c r="T29" s="12"/>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B30" s="11"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="25"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
       <c r="J30" s="12"/>
       <c r="L30" s="11"/>
       <c r="M30" s="13"/>
@@ -1393,15 +1447,15 @@
       <c r="S30" s="18"/>
       <c r="T30" s="12"/>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" s="11"/>
       <c r="C31" s="13"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="12"/>
       <c r="L31" s="11"/>
       <c r="M31" s="13"/>
@@ -1413,7 +1467,7 @@
       <c r="S31" s="18"/>
       <c r="T31" s="12"/>
     </row>
-    <row r="32" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -1433,15 +1487,15 @@
       <c r="S32" s="16"/>
       <c r="T32" s="17"/>
     </row>
-    <row r="33" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="2:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B34" s="8"/>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="20"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -1454,7 +1508,7 @@
       </c>
       <c r="N34" s="20"/>
       <c r="O34" s="9" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
@@ -1462,14 +1516,14 @@
       <c r="S34" s="9"/>
       <c r="T34" s="10"/>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B35" s="11"/>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="21"/>
+      <c r="D35" s="26"/>
       <c r="E35" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1482,7 +1536,7 @@
       </c>
       <c r="N35" s="21"/>
       <c r="O35" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
@@ -1490,12 +1544,12 @@
       <c r="S35" s="2"/>
       <c r="T35" s="12"/>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B36" s="11"/>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="22"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
@@ -1514,7 +1568,7 @@
       <c r="S36" s="13"/>
       <c r="T36" s="12"/>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
       <c r="C37" s="14"/>
       <c r="D37" s="3" t="s">
@@ -1542,47 +1596,47 @@
       <c r="S37" s="1"/>
       <c r="T37" s="12"/>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B38" s="11"/>
       <c r="C38" s="13"/>
-      <c r="D38" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="19"/>
+      <c r="D38" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="25"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
       <c r="J38" s="12"/>
       <c r="L38" s="11"/>
       <c r="M38" s="13"/>
-      <c r="N38" s="18" t="s">
-        <v>15</v>
+      <c r="N38" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="O38" s="18"/>
       <c r="P38" s="19"/>
       <c r="Q38" s="5"/>
-      <c r="R38" s="18" t="s">
-        <v>15</v>
-      </c>
+      <c r="R38" s="18"/>
       <c r="S38" s="18"/>
       <c r="T38" s="12"/>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B39" s="11"/>
       <c r="C39" s="13"/>
-      <c r="D39" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="19"/>
+      <c r="D39" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
       <c r="G39" s="5"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
       <c r="J39" s="12"/>
       <c r="L39" s="11"/>
       <c r="M39" s="13"/>
-      <c r="N39" s="18"/>
+      <c r="N39" s="28" t="s">
+        <v>41</v>
+      </c>
       <c r="O39" s="18"/>
       <c r="P39" s="19"/>
       <c r="Q39" s="7"/>
@@ -1590,39 +1644,43 @@
       <c r="S39" s="18"/>
       <c r="T39" s="12"/>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B40" s="11"/>
       <c r="C40" s="13"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="19"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
       <c r="J40" s="12"/>
       <c r="L40" s="11"/>
       <c r="M40" s="13"/>
-      <c r="N40" s="18"/>
+      <c r="N40" s="28" t="s">
+        <v>34</v>
+      </c>
       <c r="O40" s="18"/>
       <c r="P40" s="19"/>
       <c r="Q40" s="5"/>
-      <c r="R40" s="18"/>
+      <c r="R40" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="S40" s="18"/>
       <c r="T40" s="12"/>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B41" s="11"/>
       <c r="C41" s="13"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="19"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="25"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
       <c r="J41" s="12"/>
       <c r="L41" s="11"/>
       <c r="M41" s="13"/>
-      <c r="N41" s="18"/>
+      <c r="N41" s="28"/>
       <c r="O41" s="18"/>
       <c r="P41" s="19"/>
       <c r="Q41" s="5"/>
@@ -1630,19 +1688,19 @@
       <c r="S41" s="18"/>
       <c r="T41" s="12"/>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B42" s="11"/>
       <c r="C42" s="13"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="19"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="25"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
       <c r="J42" s="12"/>
       <c r="L42" s="11"/>
       <c r="M42" s="13"/>
-      <c r="N42" s="18"/>
+      <c r="N42" s="28"/>
       <c r="O42" s="18"/>
       <c r="P42" s="19"/>
       <c r="Q42" s="5"/>
@@ -1650,15 +1708,15 @@
       <c r="S42" s="18"/>
       <c r="T42" s="12"/>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B43" s="11"/>
       <c r="C43" s="13"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="19"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="25"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
       <c r="J43" s="12"/>
       <c r="L43" s="11"/>
       <c r="M43" s="13"/>
@@ -1670,15 +1728,15 @@
       <c r="S43" s="18"/>
       <c r="T43" s="12"/>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B44" s="11"/>
       <c r="C44" s="13"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="19"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="25"/>
       <c r="G44" s="5"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
       <c r="J44" s="12"/>
       <c r="L44" s="11"/>
       <c r="M44" s="13"/>
@@ -1690,15 +1748,15 @@
       <c r="S44" s="18"/>
       <c r="T44" s="12"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B45" s="11"/>
       <c r="C45" s="13"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="19"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="25"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
       <c r="J45" s="12"/>
       <c r="L45" s="11"/>
       <c r="M45" s="13"/>
@@ -1710,15 +1768,15 @@
       <c r="S45" s="18"/>
       <c r="T45" s="12"/>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B46" s="11"/>
       <c r="C46" s="13"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="25"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
       <c r="J46" s="12"/>
       <c r="L46" s="11"/>
       <c r="M46" s="13"/>
@@ -1730,15 +1788,15 @@
       <c r="S46" s="18"/>
       <c r="T46" s="12"/>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B47" s="11"/>
       <c r="C47" s="13"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="6"/>
       <c r="G47" s="5"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
       <c r="J47" s="12"/>
       <c r="L47" s="11"/>
       <c r="M47" s="13"/>
@@ -1750,7 +1808,7 @@
       <c r="S47" s="18"/>
       <c r="T47" s="12"/>
     </row>
-    <row r="48" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="15"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -1770,96 +1828,201 @@
       <c r="S48" s="16"/>
       <c r="T48" s="17"/>
     </row>
+    <row r="49" spans="12:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="12:20" ht="21" x14ac:dyDescent="0.4">
+      <c r="L50" s="8"/>
+      <c r="M50" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="N50" s="20"/>
+      <c r="O50" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="10"/>
+    </row>
+    <row r="51" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L51" s="11"/>
+      <c r="M51" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N51" s="21"/>
+      <c r="O51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="12"/>
+    </row>
+    <row r="52" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L52" s="11"/>
+      <c r="M52" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="N52" s="22"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="13"/>
+      <c r="T52" s="12"/>
+    </row>
+    <row r="53" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L53" s="11"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O53" s="1"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S53" s="1"/>
+      <c r="T53" s="12"/>
+    </row>
+    <row r="54" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L54" s="11"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="O54" s="18"/>
+      <c r="P54" s="19"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="S54" s="18"/>
+      <c r="T54" s="12"/>
+    </row>
+    <row r="55" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L55" s="11"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="19"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="12"/>
+    </row>
+    <row r="56" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L56" s="11"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="19"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="12"/>
+    </row>
+    <row r="57" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L57" s="11"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="12"/>
+    </row>
+    <row r="58" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L58" s="11"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="19"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="18"/>
+      <c r="S58" s="18"/>
+      <c r="T58" s="12"/>
+    </row>
+    <row r="59" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L59" s="11"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="19"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="18"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="12"/>
+    </row>
+    <row r="60" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L60" s="11"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="19"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="18"/>
+      <c r="S60" s="18"/>
+      <c r="T60" s="12"/>
+    </row>
+    <row r="61" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L61" s="11"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="19"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+      <c r="T61" s="12"/>
+    </row>
+    <row r="62" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L62" s="11"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="19"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="18"/>
+      <c r="S62" s="18"/>
+      <c r="T62" s="12"/>
+    </row>
+    <row r="63" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L63" s="11"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="18"/>
+      <c r="S63" s="18"/>
+      <c r="T63" s="12"/>
+    </row>
+    <row r="64" spans="12:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L64" s="15"/>
+      <c r="M64" s="16"/>
+      <c r="N64" s="16"/>
+      <c r="O64" s="16"/>
+      <c r="P64" s="16"/>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
+      <c r="T64" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="132">
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="N46:P46"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="N43:P43"/>
-    <mergeCell ref="R43:S43"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="R45:S45"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="R41:S41"/>
-    <mergeCell ref="N42:P42"/>
-    <mergeCell ref="R42:S42"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="R6:S6"/>
+  <mergeCells count="88">
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D9:F9"/>
@@ -1873,37 +2036,72 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="H44:I44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1911,12 +2109,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2103,15 +2298,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8839EA78-D391-4E41-928F-D5ECCA85A531}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEC08E90-DD5C-4C0C-87A8-09D255D174F1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="86ce603d-f463-4e75-b7e9-131a97709bff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="64124355-cabc-4b7d-957b-ceba7f756cb5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2136,18 +2343,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEC08E90-DD5C-4C0C-87A8-09D255D174F1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8839EA78-D391-4E41-928F-D5ECCA85A531}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="86ce603d-f463-4e75-b7e9-131a97709bff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="64124355-cabc-4b7d-957b-ceba7f756cb5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>